<commit_message>
Format report emails as html
 On branch html
 Changes to be committed:
	modified:   demo/Examen_final_GCHdemo_2021.xlsx
	modified:   demo/demo_correction_basic.ipynb
	modified:   transparent_correction.py
</commit_message>
<xml_diff>
--- a/demo/Examen_final_GCHdemo_2021.xlsx
+++ b/demo/Examen_final_GCHdemo_2021.xlsx
@@ -10,14 +10,15 @@
     <sheet name="notes_totales" sheetId="1" r:id="rId1"/>
     <sheet name="detail" sheetId="2" r:id="rId2"/>
     <sheet name="codes_pondération" sheetId="3" r:id="rId3"/>
-    <sheet name="erreurs" sheetId="4" r:id="rId4"/>
+    <sheet name="fréquence_erreurs" sheetId="4" r:id="rId4"/>
+    <sheet name="erreurs" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="25">
   <si>
     <t>prénom</t>
   </si>
@@ -89,6 +90,9 @@
   </si>
   <si>
     <t>réponse manquante (la question n'a pas été faite)</t>
+  </si>
+  <si>
+    <t>fréquence erreurs (%)</t>
   </si>
 </sst>
 </file>
@@ -650,6 +654,97 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2">
+        <v>100</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3">
+        <v>50</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4">
+        <v>50</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5">
+        <v>50</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6">
+        <v>50</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>